<commit_message>
Fix typos in taxonomic names
</commit_message>
<xml_diff>
--- a/data/ecocean/Donnees peches Girel 2013.xlsx
+++ b/data/ecocean/Donnees peches Girel 2013.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Desktop\medplanet\data\ecocean\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiho/Work/projects/medplanet/data/ecocean/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="26080" yWindow="460" windowWidth="25120" windowHeight="28340"/>
   </bookViews>
   <sheets>
     <sheet name="Girel 2013 propre" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -107,9 +110,6 @@
     <t>zone D</t>
   </si>
   <si>
-    <t>Blennidae</t>
-  </si>
-  <si>
     <t>parasité</t>
   </si>
   <si>
@@ -179,9 +179,6 @@
     <t>30 +-</t>
   </si>
   <si>
-    <t>Scorpenidae</t>
-  </si>
-  <si>
     <t>200+-</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t>Carangidae</t>
   </si>
   <si>
-    <t>Mulidae</t>
-  </si>
-  <si>
     <t>50 +-</t>
   </si>
   <si>
@@ -239,9 +233,6 @@
     <t>carangidae</t>
   </si>
   <si>
-    <t>blennidae</t>
-  </si>
-  <si>
     <t>MARSEILLE</t>
   </si>
   <si>
@@ -263,21 +254,12 @@
     <t>Parablennius</t>
   </si>
   <si>
-    <t xml:space="preserve">Gaidrosparus </t>
-  </si>
-  <si>
     <t>mediterraneus</t>
   </si>
   <si>
-    <t xml:space="preserve">Pagelus </t>
-  </si>
-  <si>
     <t>acarne</t>
   </si>
   <si>
-    <t>Pagelus</t>
-  </si>
-  <si>
     <t>salpa</t>
   </si>
   <si>
@@ -293,9 +275,6 @@
     <t>pilchardus</t>
   </si>
   <si>
-    <t>surmulletus</t>
-  </si>
-  <si>
     <t>Mullus</t>
   </si>
   <si>
@@ -387,6 +366,30 @@
   </si>
   <si>
     <t>vers sp2</t>
+  </si>
+  <si>
+    <t>Scorpaenidae</t>
+  </si>
+  <si>
+    <t>gaidropsarus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gaidropsarus </t>
+  </si>
+  <si>
+    <t>mullidae</t>
+  </si>
+  <si>
+    <t>blenniidae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pagellus </t>
+  </si>
+  <si>
+    <t>pagellus</t>
+  </si>
+  <si>
+    <t>surmuletus</t>
   </si>
 </sst>
 </file>
@@ -613,7 +616,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -877,44 +880,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F76" workbookViewId="0">
-      <selection activeCell="P91" sqref="P91"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.42578125" style="20"/>
-    <col min="7" max="7" width="11.42578125" style="19"/>
-    <col min="10" max="10" width="11.42578125" style="30"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" style="34" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" style="34"/>
+    <col min="3" max="3" width="10.83203125" style="20"/>
+    <col min="7" max="7" width="10.83203125" style="19"/>
+    <col min="10" max="10" width="10.83203125" style="30"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" style="34" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" style="34"/>
     <col min="16" max="16" width="18" style="16" customWidth="1"/>
-    <col min="19" max="19" width="11.42578125" style="30"/>
-    <col min="20" max="20" width="11.42578125" style="5"/>
+    <col min="19" max="19" width="10.83203125" style="30"/>
+    <col min="20" max="20" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="M1" s="39"/>
       <c r="N1" s="39"/>
       <c r="Q1" s="8" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="S1" s="40"/>
       <c r="U1" s="8" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="V1" s="8" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="X1" s="8" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="Y1" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -994,24 +997,24 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G3" s="25">
         <v>41409</v>
@@ -1023,10 +1026,10 @@
         <v>7</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>27</v>
+        <v>117</v>
       </c>
       <c r="M3" s="33" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="O3" s="36">
         <v>2</v>
@@ -1038,28 +1041,28 @@
         <v>25</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="T3" s="10"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G4" s="25">
         <v>41409</v>
@@ -1071,13 +1074,13 @@
         <v>7</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M4" s="33" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="N4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="O4" s="36">
         <v>1</v>
@@ -1090,24 +1093,24 @@
       </c>
       <c r="T4" s="10"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G5" s="25">
         <v>41409</v>
@@ -1119,13 +1122,13 @@
         <v>7</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M5" s="33" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="N5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="O5" s="36">
         <v>1</v>
@@ -1138,24 +1141,24 @@
       </c>
       <c r="T5" s="10"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G6" s="25">
         <v>41409</v>
@@ -1167,7 +1170,7 @@
         <v>7</v>
       </c>
       <c r="L6" s="33" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M6" s="33"/>
       <c r="O6" s="36">
@@ -1181,24 +1184,24 @@
       </c>
       <c r="T6" s="10"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G7" s="25">
         <v>41409</v>
@@ -1210,7 +1213,7 @@
         <v>7</v>
       </c>
       <c r="L7" s="33" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="M7" s="33"/>
       <c r="O7" s="36">
@@ -1224,24 +1227,24 @@
       </c>
       <c r="T7" s="10"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G8" s="25">
         <v>41409</v>
@@ -1253,7 +1256,7 @@
         <v>7</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="M8" s="33"/>
       <c r="O8" s="22">
@@ -1267,24 +1270,24 @@
       </c>
       <c r="T8" s="10"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G9" s="25">
         <v>41415</v>
@@ -1296,7 +1299,7 @@
         <v>5</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M9" s="33"/>
       <c r="O9" s="36">
@@ -1310,24 +1313,24 @@
       </c>
       <c r="T9" s="10"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G10" s="25">
         <v>41415</v>
@@ -1339,7 +1342,7 @@
         <v>5</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M10" s="33"/>
       <c r="O10" s="36">
@@ -1352,27 +1355,27 @@
         <v>60</v>
       </c>
       <c r="S10" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G11" s="25">
         <v>41415</v>
@@ -1384,11 +1387,11 @@
         <v>5</v>
       </c>
       <c r="L11" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M11" s="33"/>
       <c r="O11" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P11" s="22">
         <v>0</v>
@@ -1396,24 +1399,24 @@
       <c r="Q11" s="11"/>
       <c r="T11" s="10"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G12" s="26">
         <v>41429</v>
@@ -1425,13 +1428,13 @@
         <v>8</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M12" s="33" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="N12" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="O12" s="37">
         <v>1</v>
@@ -1444,24 +1447,24 @@
       </c>
       <c r="T12" s="31"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G13" s="26">
         <v>41429</v>
@@ -1473,7 +1476,7 @@
         <v>8</v>
       </c>
       <c r="L13" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M13" s="33"/>
       <c r="O13" s="37">
@@ -1485,24 +1488,24 @@
       <c r="Q13" s="37"/>
       <c r="T13" s="6"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G14" s="26">
         <v>41429</v>
@@ -1514,7 +1517,7 @@
         <v>8</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M14" s="33"/>
       <c r="O14" s="37">
@@ -1528,24 +1531,24 @@
       </c>
       <c r="T14" s="6"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G15" s="26">
         <v>41429</v>
@@ -1557,7 +1560,7 @@
         <v>8</v>
       </c>
       <c r="L15" s="22" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="M15" s="33"/>
       <c r="O15" s="28">
@@ -1571,24 +1574,24 @@
       </c>
       <c r="T15" s="6"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G16" s="26">
         <v>41430</v>
@@ -1600,7 +1603,7 @@
         <v>6</v>
       </c>
       <c r="L16" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M16" s="33"/>
       <c r="O16" s="37">
@@ -1614,24 +1617,24 @@
       </c>
       <c r="T16" s="6"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G17" s="26">
         <v>41430</v>
@@ -1643,7 +1646,7 @@
         <v>6</v>
       </c>
       <c r="L17" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M17" s="33"/>
       <c r="O17" s="37">
@@ -1655,24 +1658,24 @@
       <c r="Q17" s="14"/>
       <c r="T17" s="6"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G18" s="26">
         <v>41433</v>
@@ -1684,7 +1687,7 @@
         <v>8</v>
       </c>
       <c r="L18" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M18" s="33"/>
       <c r="O18" s="37">
@@ -1697,27 +1700,27 @@
         <v>15</v>
       </c>
       <c r="S18" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G19" s="26">
         <v>41433</v>
@@ -1729,13 +1732,13 @@
         <v>8</v>
       </c>
       <c r="L19" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M19" s="33" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="N19" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="O19" s="37">
         <v>1</v>
@@ -1747,28 +1750,28 @@
         <v>30</v>
       </c>
       <c r="S19" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T19" s="6"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G20" s="26">
         <v>41433</v>
@@ -1780,13 +1783,13 @@
         <v>8</v>
       </c>
       <c r="L20" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M20" s="33" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="N20" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="O20" s="37">
         <v>1</v>
@@ -1799,24 +1802,24 @@
       </c>
       <c r="T20" s="6"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G21" s="26">
         <v>41433</v>
@@ -1828,11 +1831,11 @@
         <v>8</v>
       </c>
       <c r="L21" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M21" s="33"/>
       <c r="O21" s="28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P21" s="15">
         <v>0</v>
@@ -1842,24 +1845,24 @@
       </c>
       <c r="T21" s="6"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G22" s="26">
         <v>41433</v>
@@ -1871,7 +1874,7 @@
         <v>8</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M22" s="33"/>
       <c r="O22" s="28">
@@ -1883,24 +1886,24 @@
       <c r="Q22" s="14"/>
       <c r="T22" s="6"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G23" s="26">
         <v>41434</v>
@@ -1912,7 +1915,7 @@
         <v>8</v>
       </c>
       <c r="L23" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M23" s="33"/>
       <c r="O23" s="37">
@@ -1924,24 +1927,24 @@
       <c r="Q23" s="14"/>
       <c r="T23" s="6"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G24" s="26">
         <v>41434</v>
@@ -1953,7 +1956,7 @@
         <v>8</v>
       </c>
       <c r="L24" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M24" s="33"/>
       <c r="O24" s="37">
@@ -1967,24 +1970,24 @@
       </c>
       <c r="T24" s="6"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G25" s="26">
         <v>41435</v>
@@ -1996,7 +1999,7 @@
         <v>8</v>
       </c>
       <c r="L25" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M25" s="33"/>
       <c r="O25" s="37">
@@ -2008,24 +2011,24 @@
       <c r="Q25" s="28"/>
       <c r="T25" s="6"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G26" s="26">
         <v>41435</v>
@@ -2037,11 +2040,11 @@
         <v>8</v>
       </c>
       <c r="L26" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M26" s="33"/>
       <c r="O26" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P26" s="15">
         <v>0</v>
@@ -2051,24 +2054,24 @@
       </c>
       <c r="T26" s="6"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G27" s="26">
         <v>41435</v>
@@ -2080,13 +2083,13 @@
         <v>8</v>
       </c>
       <c r="L27" s="22" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="M27" s="33" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="N27" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="O27" s="37">
         <v>1</v>
@@ -2099,24 +2102,24 @@
       </c>
       <c r="T27" s="6"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G28" s="26">
         <v>41435</v>
@@ -2128,10 +2131,10 @@
         <v>8</v>
       </c>
       <c r="L28" s="22" t="s">
-        <v>27</v>
+        <v>117</v>
       </c>
       <c r="M28" s="33" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="O28" s="37">
         <v>3</v>
@@ -2144,24 +2147,24 @@
       </c>
       <c r="T28" s="6"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G29" s="26">
         <v>41435</v>
@@ -2173,13 +2176,13 @@
         <v>8</v>
       </c>
       <c r="L29" s="22" t="s">
-        <v>27</v>
+        <v>117</v>
       </c>
       <c r="M29" s="33" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="N29" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O29" s="37">
         <v>1</v>
@@ -2191,27 +2194,27 @@
         <v>10</v>
       </c>
       <c r="S29" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G30" s="26">
         <v>41435</v>
@@ -2223,10 +2226,10 @@
         <v>8</v>
       </c>
       <c r="L30" s="41" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="M30" s="42" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="O30" s="37">
         <v>1</v>
@@ -2239,24 +2242,24 @@
       </c>
       <c r="T30" s="6"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G31" s="26">
         <v>41435</v>
@@ -2268,7 +2271,7 @@
         <v>8</v>
       </c>
       <c r="L31" s="22" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="M31" s="33"/>
       <c r="O31" s="37">
@@ -2282,24 +2285,24 @@
       </c>
       <c r="T31" s="6"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>26</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G32" s="26">
         <v>41436</v>
@@ -2311,11 +2314,11 @@
         <v>3</v>
       </c>
       <c r="L32" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M32" s="33"/>
       <c r="O32" s="37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P32" s="15">
         <v>0</v>
@@ -2325,24 +2328,24 @@
       </c>
       <c r="T32" s="6"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>26</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G33" s="26">
         <v>41436</v>
@@ -2354,11 +2357,11 @@
         <v>3</v>
       </c>
       <c r="L33" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M33" s="33"/>
       <c r="O33" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P33" s="15">
         <v>0</v>
@@ -2366,24 +2369,24 @@
       <c r="Q33" s="28"/>
       <c r="T33" s="6"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>26</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G34" s="26">
         <v>41436</v>
@@ -2395,10 +2398,10 @@
         <v>3</v>
       </c>
       <c r="L34" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M34" s="33" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="O34" s="37">
         <v>1</v>
@@ -2411,24 +2414,24 @@
       </c>
       <c r="T34" s="6"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G35" s="26">
         <v>41437</v>
@@ -2440,7 +2443,7 @@
         <v>3</v>
       </c>
       <c r="L35" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M35" s="33"/>
       <c r="O35" s="37">
@@ -2452,24 +2455,24 @@
       <c r="Q35" s="28"/>
       <c r="T35" s="6"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G36" s="26">
         <v>41437</v>
@@ -2481,11 +2484,11 @@
         <v>3</v>
       </c>
       <c r="L36" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M36" s="33"/>
       <c r="O36" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P36" s="15">
         <v>0</v>
@@ -2495,24 +2498,24 @@
       </c>
       <c r="T36" s="6"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G37" s="26">
         <v>41437</v>
@@ -2524,13 +2527,13 @@
         <v>3</v>
       </c>
       <c r="L37" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M37" s="29" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="N37" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="O37" s="37">
         <v>1</v>
@@ -2542,28 +2545,28 @@
         <v>80</v>
       </c>
       <c r="S37" s="15" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="T37" s="32"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G38" s="26">
         <v>41437</v>
@@ -2575,13 +2578,13 @@
         <v>3</v>
       </c>
       <c r="L38" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M38" s="33" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="N38" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="O38" s="37">
         <v>1</v>
@@ -2593,28 +2596,28 @@
         <v>40</v>
       </c>
       <c r="S38" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T38" s="6"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G39" s="26">
         <v>41437</v>
@@ -2626,7 +2629,7 @@
         <v>3</v>
       </c>
       <c r="L39" s="22" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="M39" s="33"/>
       <c r="O39" s="37">
@@ -2640,24 +2643,24 @@
       </c>
       <c r="T39" s="32"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G40" s="26">
         <v>41438</v>
@@ -2669,11 +2672,11 @@
         <v>7</v>
       </c>
       <c r="L40" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M40" s="33"/>
       <c r="O40" s="37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P40" s="15">
         <v>0</v>
@@ -2683,24 +2686,24 @@
       </c>
       <c r="T40" s="32"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F41" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G41" s="26">
         <v>41438</v>
@@ -2712,7 +2715,7 @@
         <v>7</v>
       </c>
       <c r="L41" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M41" s="33"/>
       <c r="O41" s="37">
@@ -2724,24 +2727,24 @@
       <c r="Q41" s="28"/>
       <c r="T41" s="32"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E42" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G42" s="26">
         <v>41438</v>
@@ -2753,10 +2756,10 @@
         <v>7</v>
       </c>
       <c r="L42" s="22" t="s">
-        <v>27</v>
+        <v>117</v>
       </c>
       <c r="M42" s="33" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="O42" s="37">
         <v>1</v>
@@ -2769,24 +2772,24 @@
       </c>
       <c r="T42" s="32"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G43" s="26">
         <v>41439</v>
@@ -2798,7 +2801,7 @@
         <v>7</v>
       </c>
       <c r="L43" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M43" s="33"/>
       <c r="O43" s="37">
@@ -2812,24 +2815,24 @@
       </c>
       <c r="T43" s="32"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G44" s="26">
         <v>41439</v>
@@ -2841,11 +2844,11 @@
         <v>5</v>
       </c>
       <c r="L44" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M44" s="33"/>
       <c r="O44" s="37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P44" s="15">
         <v>0</v>
@@ -2853,24 +2856,24 @@
       <c r="Q44" s="28"/>
       <c r="T44" s="32"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G45" s="26">
         <v>41440</v>
@@ -2882,13 +2885,13 @@
         <v>6</v>
       </c>
       <c r="L45" s="22" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="M45" s="33" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="N45" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="O45" s="37">
         <v>1</v>
@@ -2900,30 +2903,30 @@
         <v>120</v>
       </c>
       <c r="S45" s="15" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="T45" s="32" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D46" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E46" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G46" s="26">
         <v>41440</v>
@@ -2935,7 +2938,7 @@
         <v>6</v>
       </c>
       <c r="L46" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M46" s="33"/>
       <c r="O46" s="37">
@@ -2949,24 +2952,24 @@
       </c>
       <c r="T46" s="32"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G47" s="26">
         <v>41440</v>
@@ -2978,11 +2981,11 @@
         <v>6</v>
       </c>
       <c r="L47" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M47" s="33"/>
       <c r="O47" s="37" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P47" s="15">
         <v>0</v>
@@ -2990,24 +2993,24 @@
       <c r="Q47" s="28"/>
       <c r="T47" s="32"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G48" s="27">
         <v>41456</v>
@@ -3019,7 +3022,7 @@
         <v>5</v>
       </c>
       <c r="L48" s="22" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="M48" s="29"/>
       <c r="O48" s="37">
@@ -3032,27 +3035,27 @@
         <v>5</v>
       </c>
       <c r="T48" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E49" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G49" s="26">
         <v>41456</v>
@@ -3064,7 +3067,7 @@
         <v>5</v>
       </c>
       <c r="L49" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M49" s="33"/>
       <c r="O49" s="37">
@@ -3078,24 +3081,24 @@
       </c>
       <c r="T49" s="12"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G50" s="26">
         <v>41456</v>
@@ -3107,11 +3110,11 @@
         <v>5</v>
       </c>
       <c r="L50" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M50" s="33"/>
       <c r="O50" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P50" s="15">
         <v>0</v>
@@ -3119,24 +3122,24 @@
       <c r="Q50" s="15"/>
       <c r="T50" s="12"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D51" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G51" s="26">
         <v>41457</v>
@@ -3148,11 +3151,11 @@
         <v>5</v>
       </c>
       <c r="L51" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M51" s="33"/>
       <c r="O51" s="28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P51" s="15">
         <v>0</v>
@@ -3160,24 +3163,24 @@
       <c r="Q51" s="15"/>
       <c r="T51" s="12"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D52" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G52" s="26">
         <v>41457</v>
@@ -3189,7 +3192,7 @@
         <v>5</v>
       </c>
       <c r="L52" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M52" s="33"/>
       <c r="O52" s="28">
@@ -3203,24 +3206,24 @@
       </c>
       <c r="T52" s="12"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D53" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G53" s="26">
         <v>41458</v>
@@ -3232,11 +3235,11 @@
         <v>7</v>
       </c>
       <c r="L53" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M53" s="33"/>
       <c r="O53" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P53" s="15">
         <v>0</v>
@@ -3246,24 +3249,24 @@
       </c>
       <c r="T53" s="12"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G54" s="26">
         <v>41458</v>
@@ -3275,11 +3278,11 @@
         <v>7</v>
       </c>
       <c r="L54" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M54" s="33"/>
       <c r="O54" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P54" s="15">
         <v>0</v>
@@ -3289,24 +3292,24 @@
       </c>
       <c r="T54" s="12"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G55" s="26">
         <v>41458</v>
@@ -3318,7 +3321,7 @@
         <v>7</v>
       </c>
       <c r="L55" s="22" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="M55" s="33"/>
       <c r="O55" s="28">
@@ -3332,24 +3335,24 @@
       </c>
       <c r="T55" s="12"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G56" s="26">
         <v>41461</v>
@@ -3361,13 +3364,13 @@
         <v>6</v>
       </c>
       <c r="L56" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M56" s="33" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="N56" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="O56" s="28">
         <v>3</v>
@@ -3379,28 +3382,28 @@
         <v>50</v>
       </c>
       <c r="S56" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T56" s="12"/>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D57" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G57" s="26">
         <v>41461</v>
@@ -3412,11 +3415,11 @@
         <v>6</v>
       </c>
       <c r="L57" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M57" s="33"/>
       <c r="O57" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P57" s="15">
         <v>0</v>
@@ -3426,24 +3429,24 @@
       </c>
       <c r="T57" s="12"/>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D58" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E58" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G58" s="26">
         <v>41461</v>
@@ -3455,11 +3458,11 @@
         <v>6</v>
       </c>
       <c r="L58" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M58" s="33"/>
       <c r="O58" s="28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P58" s="15">
         <v>0</v>
@@ -3467,24 +3470,24 @@
       <c r="Q58" s="15"/>
       <c r="T58" s="12"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D59" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F59" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G59" s="26">
         <v>41463</v>
@@ -3496,11 +3499,11 @@
         <v>5</v>
       </c>
       <c r="L59" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M59" s="33"/>
       <c r="O59" s="28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="P59" s="15">
         <v>0</v>
@@ -3510,24 +3513,24 @@
       </c>
       <c r="T59" s="12"/>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D60" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E60" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F60" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G60" s="26">
         <v>41463</v>
@@ -3539,11 +3542,11 @@
         <v>5</v>
       </c>
       <c r="L60" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M60" s="33"/>
       <c r="O60" s="28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P60" s="15">
         <v>0</v>
@@ -3551,24 +3554,24 @@
       <c r="Q60" s="15"/>
       <c r="T60" s="12"/>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D61" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G61" s="26">
         <v>41466</v>
@@ -3580,11 +3583,11 @@
         <v>3</v>
       </c>
       <c r="L61" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M61" s="33"/>
       <c r="O61" s="28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="P61" s="15">
         <v>0</v>
@@ -3594,24 +3597,24 @@
       </c>
       <c r="T61" s="12"/>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D62" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E62" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G62" s="26">
         <v>41466</v>
@@ -3623,11 +3626,11 @@
         <v>3</v>
       </c>
       <c r="L62" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M62" s="33"/>
       <c r="O62" s="28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="P62" s="15">
         <v>0</v>
@@ -3635,24 +3638,24 @@
       <c r="Q62" s="15"/>
       <c r="T62" s="12"/>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D63" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E63" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F63" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G63" s="26">
         <v>41467</v>
@@ -3664,7 +3667,7 @@
         <v>6</v>
       </c>
       <c r="L63" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M63" s="33"/>
       <c r="O63" s="28">
@@ -3678,24 +3681,24 @@
       </c>
       <c r="T63" s="12"/>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D64" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E64" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F64" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G64" s="26">
         <v>41467</v>
@@ -3707,7 +3710,7 @@
         <v>6</v>
       </c>
       <c r="L64" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M64" s="33"/>
       <c r="O64" s="28">
@@ -3721,24 +3724,24 @@
       </c>
       <c r="T64" s="12"/>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D65" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E65" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G65" s="26">
         <v>41467</v>
@@ -3750,13 +3753,13 @@
         <v>6</v>
       </c>
       <c r="L65" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M65" s="29" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="N65" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="O65" s="28">
         <v>1</v>
@@ -3769,24 +3772,24 @@
       </c>
       <c r="T65" s="12"/>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D66" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E66" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F66" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G66" s="26">
         <v>41467</v>
@@ -3798,7 +3801,7 @@
         <v>6</v>
       </c>
       <c r="L66" s="22" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="M66" s="33"/>
       <c r="O66" s="28">
@@ -3812,24 +3815,24 @@
       </c>
       <c r="T66" s="12"/>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D67" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E67" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F67" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G67" s="26">
         <v>41489</v>
@@ -3841,11 +3844,11 @@
         <v>9</v>
       </c>
       <c r="L67" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M67" s="33"/>
       <c r="O67" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P67" s="15">
         <v>0</v>
@@ -3855,24 +3858,24 @@
       </c>
       <c r="T67" s="13"/>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D68" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E68" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F68" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G68" s="26">
         <v>41489</v>
@@ -3884,7 +3887,7 @@
         <v>9</v>
       </c>
       <c r="L68" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M68" s="33"/>
       <c r="O68" s="29">
@@ -3896,24 +3899,24 @@
       <c r="Q68" s="16"/>
       <c r="T68" s="13"/>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D69" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E69" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F69" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G69" s="26">
         <v>41489</v>
@@ -3925,13 +3928,13 @@
         <v>9</v>
       </c>
       <c r="L69" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M69" s="29" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="N69" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="O69" s="29">
         <v>2</v>
@@ -3944,24 +3947,24 @@
       </c>
       <c r="T69" s="13"/>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D70" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E70" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F70" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G70" s="26">
         <v>41489</v>
@@ -3973,13 +3976,13 @@
         <v>9</v>
       </c>
       <c r="L70" s="22" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="M70" s="29" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="N70" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="O70" s="29">
         <v>1</v>
@@ -3992,24 +3995,24 @@
       </c>
       <c r="T70" s="13"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D71" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E71" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F71" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G71" s="26">
         <v>41489</v>
@@ -4021,13 +4024,13 @@
         <v>9</v>
       </c>
       <c r="L71" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M71" s="22" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="N71" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O71" s="29">
         <v>1</v>
@@ -4040,24 +4043,24 @@
       </c>
       <c r="T71" s="13"/>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A72" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D72" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E72" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F72" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G72" s="26">
         <v>41491</v>
@@ -4069,11 +4072,11 @@
         <v>9</v>
       </c>
       <c r="L72" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M72" s="29"/>
       <c r="O72" s="29" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="P72" s="15">
         <v>0</v>
@@ -4083,24 +4086,24 @@
       </c>
       <c r="T72" s="13"/>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A73" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D73" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E73" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F73" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G73" s="26">
         <v>41491</v>
@@ -4112,11 +4115,11 @@
         <v>9</v>
       </c>
       <c r="L73" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M73" s="29"/>
       <c r="O73" s="29" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P73" s="15">
         <v>0</v>
@@ -4124,24 +4127,24 @@
       <c r="Q73" s="16"/>
       <c r="T73" s="13"/>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D74" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E74" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F74" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G74" s="26">
         <v>41491</v>
@@ -4153,13 +4156,13 @@
         <v>9</v>
       </c>
       <c r="L74" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M74" s="29" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="N74" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="O74" s="29">
         <v>1</v>
@@ -4171,28 +4174,28 @@
         <v>45</v>
       </c>
       <c r="S74" s="16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="T74" s="13"/>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D75" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E75" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F75" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G75" s="26">
         <v>41491</v>
@@ -4204,13 +4207,13 @@
         <v>9</v>
       </c>
       <c r="L75" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M75" s="22" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="N75" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="O75" s="29">
         <v>2</v>
@@ -4223,24 +4226,24 @@
       </c>
       <c r="T75" s="13"/>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A76" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D76" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E76" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F76" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G76" s="26">
         <v>41491</v>
@@ -4252,10 +4255,10 @@
         <v>9</v>
       </c>
       <c r="L76" s="22" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="M76" s="29" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="O76" s="29">
         <v>1</v>
@@ -4268,24 +4271,24 @@
       </c>
       <c r="T76" s="13"/>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D77" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E77" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F77" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G77" s="26">
         <v>41491</v>
@@ -4297,7 +4300,7 @@
         <v>9</v>
       </c>
       <c r="L77" s="22" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="M77" s="29"/>
       <c r="O77" s="29">
@@ -4311,24 +4314,24 @@
       </c>
       <c r="T77" s="13"/>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D78" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E78" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F78" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G78" s="25">
         <v>41492</v>
@@ -4340,7 +4343,7 @@
         <v>9</v>
       </c>
       <c r="L78" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M78" s="22"/>
       <c r="O78" s="22">
@@ -4354,24 +4357,24 @@
       </c>
       <c r="T78" s="10"/>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A79" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D79" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E79" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F79" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G79" s="25">
         <v>41492</v>
@@ -4383,7 +4386,7 @@
         <v>9</v>
       </c>
       <c r="L79" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M79" s="22"/>
       <c r="O79" s="22">
@@ -4395,24 +4398,24 @@
       <c r="Q79" s="11"/>
       <c r="T79" s="10"/>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A80" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D80" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E80" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F80" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G80" s="25">
         <v>41492</v>
@@ -4424,13 +4427,13 @@
         <v>9</v>
       </c>
       <c r="L80" s="22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M80" s="22" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="N80" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="O80" s="22">
         <v>4</v>
@@ -4443,24 +4446,24 @@
       </c>
       <c r="T80" s="10"/>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A81" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D81" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E81" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F81" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G81" s="25">
         <v>41492</v>
@@ -4472,13 +4475,13 @@
         <v>9</v>
       </c>
       <c r="L81" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M81" s="22" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="N81" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="O81" s="22">
         <v>1</v>
@@ -4490,28 +4493,28 @@
         <v>12</v>
       </c>
       <c r="S81" s="11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="T81" s="10"/>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D82" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E82" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F82" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G82" s="25">
         <v>41492</v>
@@ -4523,10 +4526,10 @@
         <v>9</v>
       </c>
       <c r="L82" s="22" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="M82" s="22" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="O82" s="22">
         <v>1</v>
@@ -4539,24 +4542,24 @@
       </c>
       <c r="T82" s="10"/>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A83" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D83" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E83" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F83" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G83" s="25">
         <v>41492</v>
@@ -4568,13 +4571,13 @@
         <v>9</v>
       </c>
       <c r="L83" s="22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M83" s="22" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="N83" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="O83" s="22">
         <v>2</v>
@@ -4587,24 +4590,24 @@
       </c>
       <c r="T83" s="10"/>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A84" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D84" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E84" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F84" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G84" s="25">
         <v>41492</v>
@@ -4616,7 +4619,7 @@
         <v>9</v>
       </c>
       <c r="L84" s="22" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="M84" s="22"/>
       <c r="O84" s="22">
@@ -4629,27 +4632,27 @@
         <v>10</v>
       </c>
       <c r="T84" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A85" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D85" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E85" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F85" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G85" s="25">
         <v>41492</v>
@@ -4661,10 +4664,10 @@
         <v>9</v>
       </c>
       <c r="L85" s="22" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="M85" s="22" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="O85" s="22">
         <v>1</v>
@@ -4676,27 +4679,27 @@
         <v>100</v>
       </c>
       <c r="S85" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A86" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D86" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E86" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F86" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G86" s="25">
         <v>41492</v>
@@ -4708,7 +4711,7 @@
         <v>9</v>
       </c>
       <c r="L86" s="22" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="M86" s="22"/>
       <c r="O86" s="22">
@@ -4722,24 +4725,24 @@
       </c>
       <c r="T86" s="10"/>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A87" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D87" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E87" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F87" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G87" s="26">
         <v>41498</v>
@@ -4751,7 +4754,7 @@
         <v>9</v>
       </c>
       <c r="L87" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M87" s="22"/>
       <c r="O87" s="22">
@@ -4765,24 +4768,24 @@
       </c>
       <c r="T87" s="13"/>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A88" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D88" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E88" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F88" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G88" s="26">
         <v>41498</v>
@@ -4794,7 +4797,7 @@
         <v>9</v>
       </c>
       <c r="L88" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M88" s="22"/>
       <c r="O88" s="22">
@@ -4806,24 +4809,24 @@
       <c r="Q88" s="16"/>
       <c r="T88" s="13"/>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A89" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D89" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E89" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F89" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G89" s="26">
         <v>41498</v>
@@ -4835,13 +4838,13 @@
         <v>9</v>
       </c>
       <c r="L89" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M89" s="22" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="N89" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O89" s="22">
         <v>1</v>
@@ -4854,24 +4857,24 @@
       </c>
       <c r="T89" s="13"/>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A90" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D90" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E90" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F90" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G90" s="26">
         <v>41498</v>
@@ -4883,13 +4886,13 @@
         <v>9</v>
       </c>
       <c r="L90" s="22" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M90" s="22" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="N90" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="O90" s="22">
         <v>1</v>
@@ -4902,24 +4905,24 @@
       </c>
       <c r="T90" s="13"/>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A91" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D91" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E91" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F91" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G91" s="26">
         <v>41515</v>
@@ -4931,7 +4934,7 @@
         <v>5</v>
       </c>
       <c r="L91" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M91" s="22"/>
       <c r="O91" s="18">
@@ -4943,24 +4946,24 @@
       <c r="Q91" s="15"/>
       <c r="T91" s="12"/>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A92" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D92" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E92" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F92" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G92" s="26">
         <v>41515</v>
@@ -4972,7 +4975,7 @@
         <v>5</v>
       </c>
       <c r="L92" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M92" s="22"/>
       <c r="O92" s="18">
@@ -4986,24 +4989,24 @@
       </c>
       <c r="T92" s="12"/>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A93" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D93" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E93" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F93" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G93" s="26">
         <v>41515</v>
@@ -5015,13 +5018,13 @@
         <v>5</v>
       </c>
       <c r="L93" s="22" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M93" s="22" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="N93" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="O93" s="18">
         <v>1</v>
@@ -5034,24 +5037,24 @@
       </c>
       <c r="T93" s="12"/>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A94" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D94" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E94" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F94" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G94" s="26">
         <v>41516</v>
@@ -5063,7 +5066,7 @@
         <v>9</v>
       </c>
       <c r="L94" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M94" s="22"/>
       <c r="O94" s="18">
@@ -5075,24 +5078,24 @@
       <c r="Q94" s="15"/>
       <c r="T94" s="12"/>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A95" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D95" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E95" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F95" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G95" s="26">
         <v>41516</v>
@@ -5104,7 +5107,7 @@
         <v>9</v>
       </c>
       <c r="L95" s="22" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="M95" s="22"/>
       <c r="O95" s="18">
@@ -5118,24 +5121,24 @@
       </c>
       <c r="T95" s="12"/>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A96" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D96" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E96" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F96" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G96" s="26">
         <v>41516</v>
@@ -5147,13 +5150,13 @@
         <v>9</v>
       </c>
       <c r="L96" s="22" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M96" s="22" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="N96" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="O96" s="18">
         <v>1</v>
@@ -5166,24 +5169,24 @@
       </c>
       <c r="T96" s="12"/>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A97" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C97" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D97" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E97" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F97" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G97" s="27">
         <v>41518</v>
@@ -5195,13 +5198,13 @@
         <v>6</v>
       </c>
       <c r="L97" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M97" s="22" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="N97" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O97" s="18">
         <v>1</v>
@@ -5214,24 +5217,24 @@
       </c>
       <c r="T97" s="7"/>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A98" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C98" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D98" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E98" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F98" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G98" s="27">
         <v>41519</v>
@@ -5243,13 +5246,13 @@
         <v>6</v>
       </c>
       <c r="L98" s="22" t="s">
-        <v>71</v>
+        <v>117</v>
       </c>
       <c r="M98" s="22" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="N98" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O98" s="18">
         <v>1</v>

</xml_diff>